<commit_message>
Half of way to clean manufactures name
</commit_message>
<xml_diff>
--- a/datasets/sorted_manufacturers.xlsx
+++ b/datasets/sorted_manufacturers.xlsx
@@ -2293,7 +2293,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Rooyan Darou</t>
+          <t>Astrazeneca Ab</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Astrazeneca Ab</t>
+          <t>Rooyan Darou</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Ipsen</t>
+          <t>Oncotec Pharma Produktion Gmbh</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Oncotec Pharma Produktion Gmbh</t>
+          <t>Ipsen</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Sanofi Aventis</t>
+          <t>Hbm Pharma</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -2917,7 +2917,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Hbm Pharma</t>
+          <t>Takeda Italia S.p.a.</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Cipla Ltd</t>
+          <t>Sanofi Aventis</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Takeda Italia S.p.a.</t>
+          <t>Sydler</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Asa Daroo Toos</t>
+          <t>Astrazeneca</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Sydler</t>
+          <t>Excella Gmbh</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -2982,7 +2982,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Astrazeneca</t>
+          <t>Farmigea</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Excella Gmbh</t>
+          <t>Cipla Ltd</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Merck Kgaa</t>
+          <t>Asa Daroo Toos</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Farmigea</t>
+          <t>Medochemie</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Desitin</t>
+          <t>Merck Kgaa</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Medochemie</t>
+          <t>Desitin</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Imen Vaccine</t>
+          <t>F.hoffmann-la Roche</t>
         </is>
       </c>
       <c r="C214" t="n">
@@ -3216,7 +3216,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>F.hoffmann-la Roche</t>
+          <t>Imen Vaccine</t>
         </is>
       </c>
       <c r="C215" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Zydus Oncosciences</t>
+          <t>Rafarm</t>
         </is>
       </c>
       <c r="C227" t="n">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Sun Pharmaceuticals Industries Ltd</t>
+          <t>Zydus Oncosciences</t>
         </is>
       </c>
       <c r="C228" t="n">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Rafarm</t>
+          <t>Sun Pharmaceuticals Industries Ltd</t>
         </is>
       </c>
       <c r="C229" t="n">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Bausch &amp; Lomb</t>
+          <t>Generis</t>
         </is>
       </c>
       <c r="C230" t="n">
@@ -3424,7 +3424,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Nano Daru Pajuhan Pardis</t>
+          <t>Bausch &amp; Lomb</t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Generis</t>
+          <t>Nano Daru Pajuhan Pardis</t>
         </is>
       </c>
       <c r="C232" t="n">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Softgel Healthcare</t>
+          <t>TURKTIPSAN A.S.</t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -3606,7 +3606,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Bayer</t>
+          <t>Johnlee Pharmaceuticals Private Limited</t>
         </is>
       </c>
       <c r="C245" t="n">
@@ -3619,7 +3619,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>TURKTIPSAN A.S.</t>
+          <t>Softgel Healthcare</t>
         </is>
       </c>
       <c r="C246" t="n">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Hetero Labs Limited</t>
+          <t>Bayer</t>
         </is>
       </c>
       <c r="C247" t="n">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Johnlee Pharmaceuticals Private Limited</t>
+          <t>Hetero Labs Limited</t>
         </is>
       </c>
       <c r="C248" t="n">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Karfarma</t>
+          <t>BioMarin Deutschland GmbH</t>
         </is>
       </c>
       <c r="C265" t="n">
@@ -3879,7 +3879,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>BioMarin Deutschland GmbH</t>
+          <t>Karfarma</t>
         </is>
       </c>
       <c r="C266" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>polpharma sa</t>
+          <t>Serb</t>
         </is>
       </c>
       <c r="C284" t="n">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Sanofi-aventis S.p.a.</t>
+          <t>Tillomed Pharma GmbH</t>
         </is>
       </c>
       <c r="C285" t="n">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Amino Ag</t>
+          <t>polpharma sa</t>
         </is>
       </c>
       <c r="C286" t="n">
@@ -4152,7 +4152,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Serb</t>
+          <t>Tillotts Pharma</t>
         </is>
       </c>
       <c r="C287" t="n">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Tillomed Pharma GmbH</t>
+          <t>Sanofi-aventis S.p.a.</t>
         </is>
       </c>
       <c r="C288" t="n">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Tillotts Pharma</t>
+          <t>Amino Ag</t>
         </is>
       </c>
       <c r="C289" t="n">
@@ -4542,7 +4542,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Sanofi S.p.A.</t>
+          <t>Alpex Pharma Sa</t>
         </is>
       </c>
       <c r="C317" t="n">
@@ -4555,7 +4555,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Fareva (ex Pierre Fabre Medicament)</t>
+          <t>S.c. Sandoz Srl</t>
         </is>
       </c>
       <c r="C318" t="n">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Mylan Pharmaceuticals Inc</t>
+          <t>Sanofi S.p.A.</t>
         </is>
       </c>
       <c r="C319" t="n">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Plus Pharma</t>
+          <t>Fareva (ex Pierre Fabre Medicament)</t>
         </is>
       </c>
       <c r="C320" t="n">
@@ -4594,7 +4594,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Wyeth Lederle Italia S.p.a</t>
+          <t>Mylan Pharmaceuticals Inc</t>
         </is>
       </c>
       <c r="C321" t="n">
@@ -4607,7 +4607,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Alpex Pharma Sa</t>
+          <t>Plus Pharma</t>
         </is>
       </c>
       <c r="C322" t="n">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Sanofi</t>
+          <t>Wyeth Lederle Italia S.p.a</t>
         </is>
       </c>
       <c r="C323" t="n">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>S.c. Sandoz Srl</t>
+          <t>Sanofi</t>
         </is>
       </c>
       <c r="C324" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Novonordisk</t>
+          <t>Fareva Mirabel (ex Merck Sharp &amp; Dohme)</t>
         </is>
       </c>
       <c r="C325" t="n">
@@ -4659,7 +4659,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Om Pharma</t>
+          <t>Novonordisk</t>
         </is>
       </c>
       <c r="C326" t="n">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Korea United Pharma</t>
+          <t>Om Pharma</t>
         </is>
       </c>
       <c r="C327" t="n">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Fareva Mirabel (ex Merck Sharp &amp; Dohme)</t>
+          <t>Korea United Pharma</t>
         </is>
       </c>
       <c r="C328" t="n">
@@ -4984,7 +4984,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Bayer Turk Kimya</t>
+          <t>Renaudin</t>
         </is>
       </c>
       <c r="C351" t="n">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Jahanalcoholteb Arak</t>
+          <t>Virchow Drugs Limited</t>
         </is>
       </c>
       <c r="C352" t="n">
@@ -5010,7 +5010,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Catalent U.k. Swindon Zydis Limited</t>
+          <t>Bayer Turk Kimya</t>
         </is>
       </c>
       <c r="C353" t="n">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Renaudin</t>
+          <t>mahdaru Toba Nazarabad</t>
         </is>
       </c>
       <c r="C354" t="n">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Aprazer Healthcare Private Limited</t>
+          <t>Jahanalcoholteb Arak</t>
         </is>
       </c>
       <c r="C355" t="n">
@@ -5049,7 +5049,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>Virchow Drugs Limited</t>
+          <t>GAP pharmaceuticals</t>
         </is>
       </c>
       <c r="C356" t="n">
@@ -5062,7 +5062,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>mahdaru Toba Nazarabad</t>
+          <t>Catalent U.k. Swindon Zydis Limited</t>
         </is>
       </c>
       <c r="C357" t="n">
@@ -5075,7 +5075,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>Scott-Edil Pharmacia Ltd</t>
+          <t>Hk Pharma Limited</t>
         </is>
       </c>
       <c r="C358" t="n">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>GAP pharmaceuticals</t>
+          <t>Msd Schering Plough Labo</t>
         </is>
       </c>
       <c r="C359" t="n">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>Hk Pharma Limited</t>
+          <t>Laboratoires Macors</t>
         </is>
       </c>
       <c r="C360" t="n">
@@ -5114,7 +5114,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>Aspen Bad Oldesloe</t>
+          <t>Aprazer Healthcare Private Limited</t>
         </is>
       </c>
       <c r="C361" t="n">
@@ -5127,7 +5127,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>Msd Schering Plough Labo</t>
+          <t>Scott-Edil Pharmacia Ltd</t>
         </is>
       </c>
       <c r="C362" t="n">
@@ -5140,7 +5140,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>Laboratoires Macors</t>
+          <t>Aspen Bad Oldesloe</t>
         </is>
       </c>
       <c r="C363" t="n">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>Biogaran, S.A.S</t>
+          <t>Abbott Gmbh &amp; Co. Kg</t>
         </is>
       </c>
       <c r="C364" t="n">
@@ -5166,7 +5166,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>توسن دارو</t>
+          <t>Biogaran, S.A.S</t>
         </is>
       </c>
       <c r="C365" t="n">
@@ -5179,7 +5179,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>Abbott Gmbh &amp; Co. Kg</t>
+          <t>توسن دارو</t>
         </is>
       </c>
       <c r="C366" t="n">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>Reliance Industries Ltd</t>
+          <t>Ravenbhel Biotech</t>
         </is>
       </c>
       <c r="C414" t="n">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Venus Remedies</t>
+          <t>Alcon-couvreur</t>
         </is>
       </c>
       <c r="C415" t="n">
@@ -5829,7 +5829,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>Eli Lilly And Co</t>
+          <t>Reliance Industries Ltd</t>
         </is>
       </c>
       <c r="C416" t="n">
@@ -5842,7 +5842,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Std Pharmaceutical Products Ltd</t>
+          <t>Janssen-cilag</t>
         </is>
       </c>
       <c r="C417" t="n">
@@ -5855,7 +5855,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>Alphapharm Pty Ltd</t>
+          <t>Venus Remedies</t>
         </is>
       </c>
       <c r="C418" t="n">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>Ravenbhel Biotech</t>
+          <t>Mylan Laboratories Ltd</t>
         </is>
       </c>
       <c r="C419" t="n">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>Genzyme</t>
+          <t>Eli Lilly And Co</t>
         </is>
       </c>
       <c r="C420" t="n">
@@ -5894,7 +5894,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Haupt Pharma Wolfratshausen</t>
+          <t>Std Pharmaceutical Products Ltd</t>
         </is>
       </c>
       <c r="C421" t="n">
@@ -5907,7 +5907,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>Alcon-couvreur</t>
+          <t>Zydus Cadila</t>
         </is>
       </c>
       <c r="C422" t="n">
@@ -5920,7 +5920,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>Janssen-cilag</t>
+          <t>Alphapharm Pty Ltd</t>
         </is>
       </c>
       <c r="C423" t="n">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>Holopack Verpackungstechnik Gmbh</t>
+          <t>Dales Pharmaceuticals Limited</t>
         </is>
       </c>
       <c r="C424" t="n">
@@ -5946,7 +5946,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>Mylan Laboratories Ltd</t>
+          <t>Genzyme</t>
         </is>
       </c>
       <c r="C425" t="n">
@@ -5959,7 +5959,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>Zydus Cadila</t>
+          <t>Aurovitas</t>
         </is>
       </c>
       <c r="C426" t="n">
@@ -5972,7 +5972,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>taghtirkhorasan</t>
+          <t>Concord Biotech Limited</t>
         </is>
       </c>
       <c r="C427" t="n">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>PersisGen Par</t>
+          <t>Haupt Pharma Wolfratshausen</t>
         </is>
       </c>
       <c r="C428" t="n">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Dales Pharmaceuticals Limited</t>
+          <t>Intas</t>
         </is>
       </c>
       <c r="C429" t="n">
@@ -6011,7 +6011,7 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>Hanlim Pharm Co Ltd</t>
+          <t>Gufic Biosciences Ltd</t>
         </is>
       </c>
       <c r="C430" t="n">
@@ -6024,7 +6024,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>Aurovitas</t>
+          <t>Holopack Verpackungstechnik Gmbh</t>
         </is>
       </c>
       <c r="C431" t="n">
@@ -6037,7 +6037,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>Lupin Limited</t>
+          <t>taghtirkhorasan</t>
         </is>
       </c>
       <c r="C432" t="n">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>Concord Biotech Limited</t>
+          <t>PersisGen Par</t>
         </is>
       </c>
       <c r="C433" t="n">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>Intas</t>
+          <t>Hanlim Pharm Co Ltd</t>
         </is>
       </c>
       <c r="C434" t="n">
@@ -6076,7 +6076,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>Lusomedicamenta</t>
+          <t>Lupin Limited</t>
         </is>
       </c>
       <c r="C435" t="n">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>Gufic Biosciences Ltd</t>
+          <t>Lusomedicamenta</t>
         </is>
       </c>
       <c r="C436" t="n">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>LABORATOIRES COLUXIA</t>
+          <t>Ali Raif Ilac Sanayi (aris)</t>
         </is>
       </c>
       <c r="C476" t="n">
@@ -6622,7 +6622,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>Ali Raif Ilac Sanayi (aris)</t>
+          <t>LABORATOIRES COLUXIA</t>
         </is>
       </c>
       <c r="C477" t="n">
@@ -6947,7 +6947,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>Roche Pharma AG</t>
+          <t>Bag Health Care Gmbh</t>
         </is>
       </c>
       <c r="C502" t="n">
@@ -6960,7 +6960,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>I.E. Ulagay Ilac Sanayii Turk A.S.</t>
+          <t>Laboratoire Europhartech</t>
         </is>
       </c>
       <c r="C503" t="n">
@@ -6973,7 +6973,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>Nipro Pharma</t>
+          <t>Roche Pharma AG</t>
         </is>
       </c>
       <c r="C504" t="n">
@@ -6986,7 +6986,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Shimi Onsor Maryam</t>
+          <t>James Alexander Co</t>
         </is>
       </c>
       <c r="C505" t="n">
@@ -6999,7 +6999,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>Bag Health Care Gmbh</t>
+          <t>I.E. Ulagay Ilac Sanayii Turk A.S.</t>
         </is>
       </c>
       <c r="C506" t="n">
@@ -7012,7 +7012,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>Krka, D. D., Novo Mesto</t>
+          <t>CIRON DRUGS &amp; PHARMACEUTICALS PVT. LTD.</t>
         </is>
       </c>
       <c r="C507" t="n">
@@ -7025,7 +7025,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>Laboratoire Europhartech</t>
+          <t>Nipro Pharma</t>
         </is>
       </c>
       <c r="C508" t="n">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>James Alexander Co</t>
+          <t>Shimi Onsor Maryam</t>
         </is>
       </c>
       <c r="C509" t="n">
@@ -7051,7 +7051,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>SHRI HARI PHARMACEUTICALS</t>
+          <t>Excella GmbH &amp; Co. KG</t>
         </is>
       </c>
       <c r="C510" t="n">
@@ -7064,7 +7064,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>CIRON DRUGS &amp; PHARMACEUTICALS PVT. LTD.</t>
+          <t>Natco Pharma Ltd.</t>
         </is>
       </c>
       <c r="C511" t="n">
@@ -7077,7 +7077,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>Excella GmbH &amp; Co. KG</t>
+          <t>Fleet laboratories Ltd</t>
         </is>
       </c>
       <c r="C512" t="n">
@@ -7090,7 +7090,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>Beltapharm Spa</t>
+          <t>Anfarm Hellas S.A.</t>
         </is>
       </c>
       <c r="C513" t="n">
@@ -7103,7 +7103,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>Natco Pharma Ltd.</t>
+          <t>Krka, D. D., Novo Mesto</t>
         </is>
       </c>
       <c r="C514" t="n">
@@ -7116,7 +7116,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>Fleet laboratories Ltd</t>
+          <t>Snow Pharmaceuticals, LLC</t>
         </is>
       </c>
       <c r="C515" t="n">
@@ -7129,7 +7129,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>Isu Abxis</t>
+          <t>ALTAN PHARMACEUTICALS SA.</t>
         </is>
       </c>
       <c r="C516" t="n">
@@ -7142,7 +7142,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>Anfarm Hellas S.A.</t>
+          <t>SHRI HARI PHARMACEUTICALS</t>
         </is>
       </c>
       <c r="C517" t="n">
@@ -7155,7 +7155,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>Snow Pharmaceuticals, LLC</t>
+          <t>Beltapharm Spa</t>
         </is>
       </c>
       <c r="C518" t="n">
@@ -7168,7 +7168,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>Metta Life Sciences Private Limited</t>
+          <t>Esteve Quimica S.a.</t>
         </is>
       </c>
       <c r="C519" t="n">
@@ -7181,7 +7181,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>ALTAN PHARMACEUTICALS SA.</t>
+          <t>Gen Ilac</t>
         </is>
       </c>
       <c r="C520" t="n">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>Hope Pharma</t>
+          <t>Haupt Pharma Wulfing Gmbh</t>
         </is>
       </c>
       <c r="C521" t="n">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>Esteve Quimica S.a.</t>
+          <t>Isu Abxis</t>
         </is>
       </c>
       <c r="C522" t="n">
@@ -7220,7 +7220,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>Grifols Usa, Llc</t>
+          <t>Metta Life Sciences Private Limited</t>
         </is>
       </c>
       <c r="C523" t="n">
@@ -7233,7 +7233,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>Dr. Franz Khler Chemie GmbH</t>
+          <t>Hope Pharma</t>
         </is>
       </c>
       <c r="C524" t="n">
@@ -7246,7 +7246,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>Gen Ilac</t>
+          <t>Grifols Usa, Llc</t>
         </is>
       </c>
       <c r="C525" t="n">
@@ -7259,7 +7259,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>Haupt Pharma Wulfing Gmbh</t>
+          <t>Dr. Franz Khler Chemie GmbH</t>
         </is>
       </c>
       <c r="C526" t="n">

</xml_diff>

<commit_message>
finding manufacturers name per atc code
</commit_message>
<xml_diff>
--- a/datasets/sorted_manufacturers.xlsx
+++ b/datasets/sorted_manufacturers.xlsx
@@ -2917,7 +2917,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Astrazeneca</t>
+          <t>Orion</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Excella Gmbh</t>
+          <t>Astrazeneca</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Farmigea</t>
+          <t>Excella Gmbh</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Orion</t>
+          <t>World Medicine</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>World Medicine</t>
+          <t>Farmigea</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Flagship Biotech International Private Limited</t>
+          <t>Glenmark</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -3164,7 +3164,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>pourateb Gostar Iranian</t>
+          <t>Pharmathen</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Glenmark</t>
+          <t>Flagship Biotech International Private Limited</t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Pharmathen</t>
+          <t>pourateb Gostar Iranian</t>
         </is>
       </c>
       <c r="C213" t="n">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Vuab Pharma A.s.</t>
+          <t>Generis</t>
         </is>
       </c>
       <c r="C226" t="n">
@@ -3372,7 +3372,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Generis</t>
+          <t>Vuab Pharma A.s.</t>
         </is>
       </c>
       <c r="C227" t="n">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Vifor Pharma</t>
+          <t>Neon Laboratories Ltd</t>
         </is>
       </c>
       <c r="C243" t="n">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Neon Laboratories Ltd</t>
+          <t>Vifor Pharma</t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -3814,7 +3814,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Patheon</t>
+          <t>Jubilant Cadista Pharmaceuticals Inc.</t>
         </is>
       </c>
       <c r="C261" t="n">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Jubilant Cadista Pharmaceuticals Inc.</t>
+          <t>Patheon</t>
         </is>
       </c>
       <c r="C262" t="n">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Bayer Vital</t>
+          <t>Serb</t>
         </is>
       </c>
       <c r="C277" t="n">
@@ -4035,7 +4035,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Globela Pharma Pvt. Ltd.</t>
+          <t>Bayer Vital</t>
         </is>
       </c>
       <c r="C278" t="n">
@@ -4048,7 +4048,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>ROCHE</t>
+          <t>Tillomed Pharma GmbH</t>
         </is>
       </c>
       <c r="C279" t="n">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Serb</t>
+          <t>Globela Pharma Pvt. Ltd.</t>
         </is>
       </c>
       <c r="C280" t="n">
@@ -4074,7 +4074,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Tillomed Pharma GmbH</t>
+          <t>Tillotts Pharma</t>
         </is>
       </c>
       <c r="C281" t="n">
@@ -4087,7 +4087,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Tillotts Pharma</t>
+          <t>ROCHE</t>
         </is>
       </c>
       <c r="C282" t="n">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>نویا ویژن آریان</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="C284" t="n">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Laboratorio Kemex</t>
+          <t>نویا ویژن آریان</t>
         </is>
       </c>
       <c r="C285" t="n">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Laboratorio Kemex</t>
         </is>
       </c>
       <c r="C286" t="n">
@@ -4412,7 +4412,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Lundbeck</t>
+          <t>Alpex Pharma Sa</t>
         </is>
       </c>
       <c r="C307" t="n">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Alpex Pharma Sa</t>
+          <t>Lundbeck</t>
         </is>
       </c>
       <c r="C308" t="n">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Exirnanosina</t>
+          <t>Sino-swed Pharmaceutical Co.u Ltd.</t>
         </is>
       </c>
       <c r="C310" t="n">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Sino-swed Pharmaceutical Co.u Ltd.</t>
+          <t>Fareva Mirabel (ex Merck Sharp &amp; Dohme)</t>
         </is>
       </c>
       <c r="C311" t="n">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>NIRAKARA INTERNATIONAL</t>
+          <t>Exirnanosina</t>
         </is>
       </c>
       <c r="C312" t="n">
@@ -4490,7 +4490,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Fareva Mirabel (ex Merck Sharp &amp; Dohme)</t>
+          <t>NIRAKARA INTERNATIONAL</t>
         </is>
       </c>
       <c r="C313" t="n">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>Roche Pharma</t>
+          <t>Renaudin</t>
         </is>
       </c>
       <c r="C340" t="n">
@@ -4854,7 +4854,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>Renaudin</t>
+          <t>Roche Pharma</t>
         </is>
       </c>
       <c r="C341" t="n">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>Biomarin</t>
+          <t>GAP pharmaceuticals</t>
         </is>
       </c>
       <c r="C344" t="n">
@@ -4906,7 +4906,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>GAP pharmaceuticals</t>
+          <t>Hk Pharma Limited</t>
         </is>
       </c>
       <c r="C345" t="n">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Hk Pharma Limited</t>
+          <t>Msd Schering Plough Labo</t>
         </is>
       </c>
       <c r="C346" t="n">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Bipso Gmbh</t>
+          <t>Laboratoires Macors</t>
         </is>
       </c>
       <c r="C347" t="n">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>Fisiopharma</t>
+          <t>Abbott Gmbh &amp; Co. Kg</t>
         </is>
       </c>
       <c r="C348" t="n">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>Msd Schering Plough Labo</t>
+          <t>Biomarin</t>
         </is>
       </c>
       <c r="C349" t="n">
@@ -4971,7 +4971,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>RP Scherer  GmbH &amp; Co. KG</t>
+          <t>Bipso Gmbh</t>
         </is>
       </c>
       <c r="C350" t="n">
@@ -4984,7 +4984,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Laboratoires Macors</t>
+          <t>Fisiopharma</t>
         </is>
       </c>
       <c r="C351" t="n">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Piramal Healthcare Uk Limited</t>
+          <t>RP Scherer  GmbH &amp; Co. KG</t>
         </is>
       </c>
       <c r="C352" t="n">
@@ -5010,7 +5010,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Roche</t>
+          <t>Piramal Healthcare Uk Limited</t>
         </is>
       </c>
       <c r="C353" t="n">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Abbott Gmbh &amp; Co. Kg</t>
+          <t>Roche</t>
         </is>
       </c>
       <c r="C354" t="n">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>Alfasigma(ex Alfa Wassermann S.p.a.)</t>
+          <t>Reliance Life Sciences Pvt. Ltd</t>
         </is>
       </c>
       <c r="C372" t="n">
@@ -5270,7 +5270,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>United Biotech Pvt. Ltd.</t>
+          <t>Bell Pharma Pvt. Ltd.</t>
         </is>
       </c>
       <c r="C373" t="n">
@@ -5283,7 +5283,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>NuLife Pharmaceuticals</t>
+          <t>Sun Pharmaceutical</t>
         </is>
       </c>
       <c r="C374" t="n">
@@ -5296,7 +5296,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>Reliance Life Sciences Pvt. Ltd</t>
+          <t>Alfasigma(ex Alfa Wassermann S.p.a.)</t>
         </is>
       </c>
       <c r="C375" t="n">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>Bell Pharma Pvt. Ltd.</t>
+          <t>United Biotech Pvt. Ltd.</t>
         </is>
       </c>
       <c r="C376" t="n">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>Sun Pharmaceutical</t>
+          <t>NuLife Pharmaceuticals</t>
         </is>
       </c>
       <c r="C377" t="n">
@@ -5478,7 +5478,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Elfin Pvt Ltd</t>
+          <t>Ravenbhel Biotech</t>
         </is>
       </c>
       <c r="C389" t="n">
@@ -5491,7 +5491,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>نیواد فارمد سلامت</t>
+          <t>Elfin Pvt Ltd</t>
         </is>
       </c>
       <c r="C390" t="n">
@@ -5504,7 +5504,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>Glaxosmithkline Spa</t>
+          <t>Alcon-couvreur</t>
         </is>
       </c>
       <c r="C391" t="n">
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>Kyorin Pharmaceutical Co Ltd</t>
+          <t>نیواد فارمد سلامت</t>
         </is>
       </c>
       <c r="C392" t="n">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>InfoRLife SA( ex ACS Dobfar Info Sa)</t>
+          <t>Janssen-cilag</t>
         </is>
       </c>
       <c r="C393" t="n">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Ravenbhel Biotech</t>
+          <t>Glaxosmithkline Spa</t>
         </is>
       </c>
       <c r="C394" t="n">
@@ -5556,7 +5556,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Alcon-couvreur</t>
+          <t>Mylan Laboratories Ltd</t>
         </is>
       </c>
       <c r="C395" t="n">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Janssen-cilag</t>
+          <t>Kyorin Pharmaceutical Co Ltd</t>
         </is>
       </c>
       <c r="C396" t="n">
@@ -5582,7 +5582,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>B/braun</t>
+          <t>Zydus Cadila</t>
         </is>
       </c>
       <c r="C397" t="n">
@@ -5595,7 +5595,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>Mylan Laboratories Ltd</t>
+          <t>InfoRLife SA( ex ACS Dobfar Info Sa)</t>
         </is>
       </c>
       <c r="C398" t="n">
@@ -5608,7 +5608,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>Zydus Cadila</t>
+          <t>زیست فناوری کوثر</t>
         </is>
       </c>
       <c r="C399" t="n">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>IBE Pharma</t>
+          <t>Dales Pharmaceuticals Limited</t>
         </is>
       </c>
       <c r="C400" t="n">
@@ -5634,7 +5634,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>Ghadir . Co</t>
+          <t>Aurovitas</t>
         </is>
       </c>
       <c r="C401" t="n">
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>Dales Pharmaceuticals Limited</t>
+          <t>Alfasigma S.p.A</t>
         </is>
       </c>
       <c r="C402" t="n">
@@ -5660,7 +5660,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>AOP Orphan</t>
+          <t>Concord Biotech Limited</t>
         </is>
       </c>
       <c r="C403" t="n">
@@ -5673,7 +5673,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Aurovitas</t>
+          <t>Glaxo wellcome Operations</t>
         </is>
       </c>
       <c r="C404" t="n">
@@ -5686,7 +5686,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>AMW GmbH</t>
+          <t>Intas</t>
         </is>
       </c>
       <c r="C405" t="n">
@@ -5699,7 +5699,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Concord Biotech Limited</t>
+          <t>Gufic Biosciences Ltd</t>
         </is>
       </c>
       <c r="C406" t="n">
@@ -5712,7 +5712,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>H2 Pharma S.A.S</t>
+          <t>B/braun</t>
         </is>
       </c>
       <c r="C407" t="n">
@@ -5725,7 +5725,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Intas</t>
+          <t>IBE Pharma</t>
         </is>
       </c>
       <c r="C408" t="n">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Hexal</t>
+          <t>Ghadir . Co</t>
         </is>
       </c>
       <c r="C409" t="n">
@@ -5751,7 +5751,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Gufic Biosciences Ltd</t>
+          <t>AOP Orphan</t>
         </is>
       </c>
       <c r="C410" t="n">
@@ -5764,7 +5764,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Delpharm Huningue</t>
+          <t>AMW GmbH</t>
         </is>
       </c>
       <c r="C411" t="n">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Recordati S.p.a.</t>
+          <t>H2 Pharma S.A.S</t>
         </is>
       </c>
       <c r="C412" t="n">
@@ -5790,7 +5790,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>زیست فناوری کوثر</t>
+          <t>Hexal</t>
         </is>
       </c>
       <c r="C413" t="n">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>Alfasigma S.p.A</t>
+          <t>Delpharm Huningue</t>
         </is>
       </c>
       <c r="C414" t="n">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Glaxo wellcome Operations</t>
+          <t>Recordati S.p.a.</t>
         </is>
       </c>
       <c r="C415" t="n">
@@ -6180,7 +6180,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>Delpharm</t>
+          <t>Guerbet</t>
         </is>
       </c>
       <c r="C443" t="n">
@@ -6193,7 +6193,7 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>Gilead Sciences Limited</t>
+          <t>Haupt Pharma Amareg GmbH</t>
         </is>
       </c>
       <c r="C444" t="n">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>Guerbet</t>
+          <t>Bayer  Vital</t>
         </is>
       </c>
       <c r="C445" t="n">
@@ -6219,7 +6219,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>Haupt Pharma Amareg GmbH</t>
+          <t>Uriach Group</t>
         </is>
       </c>
       <c r="C446" t="n">
@@ -6232,7 +6232,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>Bayer  Vital</t>
+          <t>Delpharm</t>
         </is>
       </c>
       <c r="C447" t="n">
@@ -6245,7 +6245,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>Uriach Group</t>
+          <t>Gilead Sciences Limited</t>
         </is>
       </c>
       <c r="C448" t="n">
@@ -6557,7 +6557,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>Biogen</t>
+          <t>Bag Health Care Gmbh</t>
         </is>
       </c>
       <c r="C472" t="n">
@@ -6570,7 +6570,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>Novartis Pharma Ag</t>
+          <t>Biogen</t>
         </is>
       </c>
       <c r="C473" t="n">
@@ -6583,7 +6583,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>Thorpe Laboratories</t>
+          <t>Laboratoire Europhartech</t>
         </is>
       </c>
       <c r="C474" t="n">
@@ -6596,7 +6596,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>Qpharma Ab</t>
+          <t>Novartis Pharma Ag</t>
         </is>
       </c>
       <c r="C475" t="n">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>Bag Health Care Gmbh</t>
+          <t>James Alexander Co</t>
         </is>
       </c>
       <c r="C476" t="n">
@@ -6622,7 +6622,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>Laboratoire Europhartech</t>
+          <t>Thorpe Laboratories</t>
         </is>
       </c>
       <c r="C477" t="n">
@@ -6635,7 +6635,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>James Alexander Co</t>
+          <t>CIRON DRUGS &amp; PHARMACEUTICALS PVT. LTD.</t>
         </is>
       </c>
       <c r="C478" t="n">
@@ -6648,7 +6648,7 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>Ali Raif Ilac Sanayi (aris)</t>
+          <t>Qpharma Ab</t>
         </is>
       </c>
       <c r="C479" t="n">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>CIRON DRUGS &amp; PHARMACEUTICALS PVT. LTD.</t>
+          <t>Excella GmbH &amp; Co. KG</t>
         </is>
       </c>
       <c r="C480" t="n">
@@ -6674,7 +6674,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>Excella GmbH &amp; Co. KG</t>
+          <t>Wockhardt Limited</t>
         </is>
       </c>
       <c r="C481" t="n">
@@ -6687,7 +6687,7 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>LABORATOIRES COLUXIA</t>
+          <t>Natco Pharma Ltd.</t>
         </is>
       </c>
       <c r="C482" t="n">
@@ -6700,7 +6700,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>Ever Pharma Jena Gmbh</t>
+          <t>Fleet laboratories Ltd</t>
         </is>
       </c>
       <c r="C483" t="n">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>Natco Pharma Ltd.</t>
+          <t>LAINCO, S.A.</t>
         </is>
       </c>
       <c r="C484" t="n">
@@ -6726,7 +6726,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>Lannacher Heilittel</t>
+          <t>Anfarm Hellas S.A.</t>
         </is>
       </c>
       <c r="C485" t="n">
@@ -6739,7 +6739,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>Fleet laboratories Ltd</t>
+          <t>Cheplapharm</t>
         </is>
       </c>
       <c r="C486" t="n">
@@ -6752,7 +6752,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>Medilink A/s</t>
+          <t>Snow Pharmaceuticals, LLC</t>
         </is>
       </c>
       <c r="C487" t="n">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>Anfarm Hellas S.A.</t>
+          <t>R-pharm Germany Gmbh</t>
         </is>
       </c>
       <c r="C488" t="n">
@@ -6778,7 +6778,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>Inresa</t>
+          <t>ALTAN PHARMACEUTICALS SA.</t>
         </is>
       </c>
       <c r="C489" t="n">
@@ -6791,7 +6791,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>Snow Pharmaceuticals, LLC</t>
+          <t>Aventis Pharma Ltd</t>
         </is>
       </c>
       <c r="C490" t="n">
@@ -6804,7 +6804,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>ALTAN PHARMACEUTICALS SA.</t>
+          <t>Esteve Quimica S.a.</t>
         </is>
       </c>
       <c r="C491" t="n">
@@ -6817,7 +6817,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>Wockhardt Limited</t>
+          <t>Wasserburger Arzneimittelwerk Gmbh</t>
         </is>
       </c>
       <c r="C492" t="n">
@@ -6830,7 +6830,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>LAINCO, S.A.</t>
+          <t>Ali Raif Ilac Sanayi (aris)</t>
         </is>
       </c>
       <c r="C493" t="n">
@@ -6843,7 +6843,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>Cheplapharm</t>
+          <t>Gen Ilac</t>
         </is>
       </c>
       <c r="C494" t="n">
@@ -6856,7 +6856,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>R-pharm Germany Gmbh</t>
+          <t>Haupt Pharma Wulfing Gmbh</t>
         </is>
       </c>
       <c r="C495" t="n">
@@ -6869,7 +6869,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>Aventis Pharma Ltd</t>
+          <t>LABORATOIRES COLUXIA</t>
         </is>
       </c>
       <c r="C496" t="n">
@@ -6882,7 +6882,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>Wasserburger Arzneimittelwerk Gmbh</t>
+          <t>Ever Pharma Jena Gmbh</t>
         </is>
       </c>
       <c r="C497" t="n">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>Tty Biopharm Co Ltd</t>
+          <t>Lannacher Heilittel</t>
         </is>
       </c>
       <c r="C498" t="n">
@@ -6908,7 +6908,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>Esteve Quimica S.a.</t>
+          <t>Medilink A/s</t>
         </is>
       </c>
       <c r="C499" t="n">
@@ -6921,7 +6921,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>Ranbaxy</t>
+          <t>Inresa</t>
         </is>
       </c>
       <c r="C500" t="n">
@@ -6934,7 +6934,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>Gen Ilac</t>
+          <t>Tty Biopharm Co Ltd</t>
         </is>
       </c>
       <c r="C501" t="n">
@@ -6947,7 +6947,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>Synerlab - Laboratoires Btt</t>
+          <t>Ranbaxy</t>
         </is>
       </c>
       <c r="C502" t="n">
@@ -6960,7 +6960,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>Haupt Pharma Wulfing Gmbh</t>
+          <t>Synerlab - Laboratoires Btt</t>
         </is>
       </c>
       <c r="C503" t="n">
@@ -7389,7 +7389,7 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>Ipca Laboratories Ltd</t>
+          <t>Novartis Pharma</t>
         </is>
       </c>
       <c r="C536" t="n">
@@ -7402,7 +7402,7 @@
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>Hofmann &amp; Sommer</t>
+          <t>RECIPHARM MONTS</t>
         </is>
       </c>
       <c r="C537" t="n">
@@ -7415,7 +7415,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>SamanDaroo8</t>
+          <t>Genentech Inc</t>
         </is>
       </c>
       <c r="C538" t="n">
@@ -7428,7 +7428,7 @@
       </c>
       <c r="B539" t="inlineStr">
         <is>
-          <t>Bharat Serum and Vaccines Ltd</t>
+          <t>Lg Chem(life Sciences Company)</t>
         </is>
       </c>
       <c r="C539" t="n">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>Synthon</t>
+          <t>HRA Pharma</t>
         </is>
       </c>
       <c r="C540" t="n">
@@ -7454,7 +7454,7 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>Clausen</t>
+          <t>Atabay Kimya Sanayi Ve Ticaret As</t>
         </is>
       </c>
       <c r="C541" t="n">
@@ -7467,7 +7467,7 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>Sanquin</t>
+          <t>Ildong Pharmaceutical</t>
         </is>
       </c>
       <c r="C542" t="n">
@@ -7480,7 +7480,7 @@
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>Intas Pharmaceuticals Ltd</t>
+          <t>Sandoz Gmbh</t>
         </is>
       </c>
       <c r="C543" t="n">
@@ -7493,7 +7493,7 @@
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>Samyang</t>
+          <t>Exelead</t>
         </is>
       </c>
       <c r="C544" t="n">
@@ -7506,7 +7506,7 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>Novartis Pharma</t>
+          <t>Ipca Laboratories Ltd</t>
         </is>
       </c>
       <c r="C545" t="n">
@@ -7519,7 +7519,7 @@
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>RECIPHARM MONTS</t>
+          <t>Hofmann &amp; Sommer</t>
         </is>
       </c>
       <c r="C546" t="n">
@@ -7532,7 +7532,7 @@
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>Genentech Inc</t>
+          <t>SamanDaroo8</t>
         </is>
       </c>
       <c r="C547" t="n">
@@ -7545,7 +7545,7 @@
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>Lg Chem(life Sciences Company)</t>
+          <t>Bharat Serum and Vaccines Ltd</t>
         </is>
       </c>
       <c r="C548" t="n">
@@ -7558,7 +7558,7 @@
       </c>
       <c r="B549" t="inlineStr">
         <is>
-          <t>HRA Pharma</t>
+          <t>Synthon</t>
         </is>
       </c>
       <c r="C549" t="n">
@@ -7571,7 +7571,7 @@
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>Atabay Kimya Sanayi Ve Ticaret As</t>
+          <t>Clausen</t>
         </is>
       </c>
       <c r="C550" t="n">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>Ildong Pharmaceutical</t>
+          <t>Sanquin</t>
         </is>
       </c>
       <c r="C551" t="n">
@@ -7597,7 +7597,7 @@
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>Sandoz Gmbh</t>
+          <t>Intas Pharmaceuticals Ltd</t>
         </is>
       </c>
       <c r="C552" t="n">
@@ -7610,7 +7610,7 @@
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>Exelead</t>
+          <t>Samyang</t>
         </is>
       </c>
       <c r="C553" t="n">

</xml_diff>